<commit_message>
fixed save origin test
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/tested_state_original_design.xlsx
+++ b/dynamics/src/dynamics/xlsx/tested_state_original_design.xlsx
@@ -496,19 +496,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>122.5522352790247</v>
+        <v>176.3651844588868</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F3" t="n">
-        <v>0.02071574340946317</v>
+        <v>0.008352056178274002</v>
       </c>
       <c r="G3" t="n">
         <v>26.036</v>
@@ -536,13 +536,13 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>334.8033755635122</v>
+        <v>378.9637784732679</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F4" t="n">
-        <v>0.02071574340946317</v>
+        <v>0.008352056178274002</v>
       </c>
       <c r="G4" t="n">
         <v>26.036</v>
@@ -632,19 +632,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>232.9487758086098</v>
+        <v>328.1082605273225</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F7" t="n">
-        <v>0.02071574340946317</v>
+        <v>0.008352056178274002</v>
       </c>
       <c r="G7" t="n">
         <v>26.036</v>
@@ -672,13 +672,13 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>641.3008763241133</v>
+        <v>714.3960623361766</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F8" t="n">
-        <v>0.02071574340946317</v>
+        <v>0.008352056178274002</v>
       </c>
       <c r="G8" t="n">
         <v>26.036</v>
@@ -768,19 +768,19 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11" t="n">
-        <v>343.8415552358288</v>
+        <v>481.9949231290301</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F11" t="n">
-        <v>0.02071574340946317</v>
+        <v>0.008352056178274002</v>
       </c>
       <c r="G11" t="n">
         <v>26.036</v>
@@ -805,16 +805,16 @@
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>949.2745169019869</v>
+        <v>1053.149130220529</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F12" t="n">
-        <v>0.02071574340946317</v>
+        <v>0.008352056178274002</v>
       </c>
       <c r="G12" t="n">
         <v>26.036</v>
@@ -904,19 +904,19 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C15" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D15" t="n">
-        <v>399.6321996711864</v>
+        <v>559.0635379518063</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F15" t="n">
-        <v>0.02071574340946317</v>
+        <v>0.008352056178274002</v>
       </c>
       <c r="G15" t="n">
         <v>26.036</v>
@@ -941,16 +941,16 @@
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D16" t="n">
-        <v>1103.463822858034</v>
+        <v>1222.999659563553</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F16" t="n">
-        <v>0.02071574340946317</v>
+        <v>0.008352056178274002</v>
       </c>
       <c r="G16" t="n">
         <v>26.036</v>

</xml_diff>